<commit_message>
adding rest of the products 3
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18075" windowHeight="5070" tabRatio="619" firstSheet="25" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18075" windowHeight="5070" tabRatio="619" firstSheet="22" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="corn_bageta" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="337">
   <si>
     <t>Maslová Majoneza</t>
   </si>
@@ -1014,9 +1014,6 @@
     <t>majonéza chrenová 16,39 %</t>
   </si>
   <si>
-    <t>šunka zaúdená 18,03 %</t>
-  </si>
-  <si>
     <t>kápia sterilizovaná 4,92 %</t>
   </si>
   <si>
@@ -1116,9 +1113,6 @@
     <t>PŠENIČNÁ múka, pitná voda, pekárska zmes (10%) (slnečnica, PŠENIČNÉ otruby, ľan, ŠPALDOVÉ vločky (5,5%), pražený JAČMEŇ a RAŽ, PŠENIČNÉ vločky), ŠPALDOVÁ múka (4,5%), droždie, jedlá soľ s jódom (jedlá soľ, jodičnan draselný), repkový olej, PŠENIČNÝ GLUTÉN, emulgátor: E472e, cukor, múku upravujúca látka (E300, E920), RAŽNÁ múka.</t>
   </si>
   <si>
-    <t xml:space="preserve">Kuracie prsia 70 %, pitná voda, PŠENIČNÁ múka, rastlinný olej (BAVLNÍKOVÝ a SÓJOVÝ olej úplne hudrogenovaný), ryžova múka, SÓJOVA bielkovina, jedlá soľ, stabilizátory" trifosforečnan sodný, dihydrogén fosforečnan sodný, maltodextrín, cukor, farbivo: kurkumin, zahusťovadlo: xantánová guma, prírodná zelerová aróma. </t>
-  </si>
-  <si>
     <t xml:space="preserve">pasterizovaná SMOTANA 78 % hm., kokosový rastinný tuk 18 % hm., sučené MLIEKO, sušná STVÁTKA, zemiakový škrob, jedlá soľ 0,5 % hm., smotanová kultúra </t>
   </si>
   <si>
@@ -1126,6 +1120,18 @@
   </si>
   <si>
     <t xml:space="preserve">pitná voda, repkový olej, modifikovaný škrob a stabilizátory (E412, E415), VAJEČNÝ prípravok (VAJEČNÉ žĺtly, jedlá soľ, maltodextrín), HORČICA (pitná voda, HORČIČNÉ SEMENO, ocot kvasný liehový, jedlá soľ, korenie), kvasný ocot liehový, jedlá soľ, koreniaci prípravok (jedlá soľ, látka zvýrazňujúca chuť a vôňu (E621), sušená zelenina (mrkva, cibuľa, petržlen, pór, ZELER), škrob, cukor, byliny a korenie (obsahuje ZELER), aróma, farbivo (E101), sušený petržlen (0,45 %), cukor, konzervant (sorban draselný). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bravčové stehno min. 55 %, pitná voda, jedlá soľ, konzervačná látka (E250), bravčové kože, modifikovaný škrob (E1422), zahusťovadlo (E407, E415), živočíšna (bravčová) bielkovina, stabilizátor (E450, E451), dextróza, zvýrazňovač chuti (E621), antioxidant (E316), extrakty korenín. </t>
+  </si>
+  <si>
+    <t>Wellness Šunka zaúdená 18,03 %</t>
+  </si>
+  <si>
+    <t>kuracie mäso(65%), rastlinný olej (bavlníkový a slnečnicový), PŠENIČNÁ múka, voda, kukuričná múka, škrob, STRÚHANKA (PŠENIČNÁ múka, jedlá soľ, droždie), jedlá soľ, stabilizátor (E450i), kypriaca látka (E450i), sušené odstredené MLIEKO, dextróza, korenie a zahusťovadlo (E412).</t>
+  </si>
+  <si>
+    <t>pšenica, mlieko, strúhanka</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1191,12 +1197,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1252,7 +1252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1280,7 +1280,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8415,7 +8414,7 @@
         <v>227</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8485,7 +8484,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8520,7 +8519,7 @@
         <v>227</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8677,7 +8676,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8747,7 +8746,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8782,7 +8781,7 @@
         <v>227</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8817,7 +8816,7 @@
         <v>227</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8941,7 +8940,7 @@
         <v>244</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9011,7 +9010,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9169,7 +9168,7 @@
         <v>227</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9204,7 +9203,7 @@
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9237,7 +9236,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9355,8 +9354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9431,42 +9430,42 @@
         <v>229</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="5" t="s">
         <v>255</v>
       </c>
       <c r="B3" s="4">
         <v>62</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G3" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>227</v>
+        <v>336</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9623,7 +9622,7 @@
         <v>227</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9658,7 +9657,7 @@
         <v>269</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9693,7 +9692,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9817,7 +9816,7 @@
         <v>244</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9852,7 +9851,7 @@
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9922,7 +9921,7 @@
         <v>227</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10081,7 +10080,7 @@
         <v>244</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10110,13 +10109,13 @@
         <v>0.3</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>315</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10186,7 +10185,7 @@
         <v>227</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10345,7 +10344,7 @@
         <v>227</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10380,7 +10379,7 @@
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10415,7 +10414,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10483,7 +10482,7 @@
         <v>227</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -10496,7 +10495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -10572,7 +10571,7 @@
         <v>227</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10607,12 +10606,12 @@
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B4" s="4">
         <v>44</v>
@@ -10636,13 +10635,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10710,7 +10709,7 @@
         <v>227</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -10907,7 +10906,7 @@
         <v>227</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10942,7 +10941,7 @@
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -10977,7 +10976,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -11012,7 +11011,7 @@
         <v>227</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -11171,7 +11170,7 @@
         <v>244</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -11206,12 +11205,12 @@
         <v>227</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" s="4">
         <v>40</v>
@@ -11241,7 +11240,7 @@
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -11325,7 +11324,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11400,33 +11399,33 @@
         <v>244</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>297</v>
+      <c r="A3" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="B3" s="4">
         <v>44</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>2.81</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G3" s="4">
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="H3" s="4">
-        <v>0</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>227</v>
@@ -11434,7 +11433,9 @@
       <c r="J3" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -11462,18 +11463,18 @@
         <v>1.3</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>227</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="4">
         <v>28</v>
@@ -11503,12 +11504,12 @@
         <v>227</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B6" s="4">
         <v>12</v>
@@ -11597,7 +11598,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B2" s="4">
         <v>750</v>
@@ -11626,7 +11627,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B3" s="4">
         <v>200</v>
@@ -11655,7 +11656,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B4" s="4">
         <v>23</v>
@@ -11684,7 +11685,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B5" s="4">
         <v>70</v>
@@ -11713,7 +11714,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B6" s="4">
         <v>50</v>
@@ -11767,7 +11768,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B8" s="4">
         <v>50</v>
@@ -11823,7 +11824,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>

</xml_diff>